<commit_message>
Subo notebook con trabajo completo, además texto del informe y excel con modelo de las tablas
</commit_message>
<xml_diff>
--- a/Taller 2/tablas.xlsx
+++ b/Taller 2/tablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1655775e314bd799/Maestría IA Aplicada/Semestre 1/Aprendizaje automático III/Talleres/Taller 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{B1D44CD4-F765-41BB-8147-D381176485D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{925301D2-235B-4229-B1D2-A3ED9EFBC323}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{B1D44CD4-F765-41BB-8147-D381176485D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3C47A0D-F7F4-4DE5-9526-C6FB8097A1DD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AD1B03CA-9232-4F2D-A5D2-63064345160B}"/>
+    <workbookView xWindow="-20610" yWindow="-2475" windowWidth="20730" windowHeight="11040" xr2:uid="{AD1B03CA-9232-4F2D-A5D2-63064345160B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="134">
   <si>
     <t>Modelo</t>
   </si>
@@ -239,45 +239,21 @@
     <t>Tendencia lineal sin estacionalidad</t>
   </si>
   <si>
-    <t>888.91</t>
-  </si>
-  <si>
     <t>Captura la tendencia general, pero deja mucha variabilidad sin explicar.</t>
   </si>
   <si>
     <t>Tendencia cuadrática</t>
   </si>
   <si>
-    <t>Tendencia con término cuadrático (x²)</t>
-  </si>
-  <si>
-    <t>589.06</t>
-  </si>
-  <si>
-    <t>Mejora considerablemente la precisión al permitir curvatura en la tendencia.</t>
-  </si>
-  <si>
     <t>Lineal estacional</t>
   </si>
   <si>
     <t>Solo estacionalidad (sin tendencia)</t>
   </si>
   <si>
-    <t>1253.44</t>
-  </si>
-  <si>
-    <t>La estacionalidad por sí sola no explica bien el comportamiento global.</t>
-  </si>
-  <si>
-    <t>Tendencia + estacionalidad (cuadrática)</t>
-  </si>
-  <si>
     <t>Modelo completo con tendencia y estacionalidad</t>
   </si>
   <si>
-    <t>204.62</t>
-  </si>
-  <si>
     <t>Es el modelo más preciso: combina tendencia y estacionalidad, ajustando mejor los patrones reales.</t>
   </si>
   <si>
@@ -290,43 +266,178 @@
     <t>RMSE (test)</t>
   </si>
   <si>
-    <t>0.9626</t>
-  </si>
-  <si>
-    <t>0.9632</t>
-  </si>
-  <si>
-    <t>511.55</t>
-  </si>
-  <si>
-    <t>0.9642</t>
-  </si>
-  <si>
-    <t>424.20</t>
-  </si>
-  <si>
-    <t>0.9654</t>
-  </si>
-  <si>
-    <t>336.80</t>
-  </si>
-  <si>
-    <t>0.9664</t>
-  </si>
-  <si>
-    <t>256.22</t>
-  </si>
-  <si>
-    <t>4899.78</t>
-  </si>
-  <si>
-    <t>16172.18</t>
-  </si>
-  <si>
-    <t>17481.59</t>
-  </si>
-  <si>
-    <t>18827.05</t>
+    <t>0.9624</t>
+  </si>
+  <si>
+    <t>632.48</t>
+  </si>
+  <si>
+    <t>0.9640</t>
+  </si>
+  <si>
+    <t>546.52</t>
+  </si>
+  <si>
+    <t>0.9657</t>
+  </si>
+  <si>
+    <t>461.49</t>
+  </si>
+  <si>
+    <t>0.9672</t>
+  </si>
+  <si>
+    <t>384.85</t>
+  </si>
+  <si>
+    <t>0.9685</t>
+  </si>
+  <si>
+    <t>320.02</t>
+  </si>
+  <si>
+    <t>3699.44</t>
+  </si>
+  <si>
+    <t>12022.38</t>
+  </si>
+  <si>
+    <t>12541.37</t>
+  </si>
+  <si>
+    <t>13040.06</t>
+  </si>
+  <si>
+    <t>844.51</t>
+  </si>
+  <si>
+    <t>Tendencia con término (x²)</t>
+  </si>
+  <si>
+    <t>Mejora la precisión al permitir curvatura en la tendencia.</t>
+  </si>
+  <si>
+    <t>1272.22</t>
+  </si>
+  <si>
+    <t>Tendencia + estacionalidad (grado 6)</t>
+  </si>
+  <si>
+    <t>190.53</t>
+  </si>
+  <si>
+    <t>10,869.87</t>
+  </si>
+  <si>
+    <t>10,459.78</t>
+  </si>
+  <si>
+    <t>11,279.95</t>
+  </si>
+  <si>
+    <t>10,838.85</t>
+  </si>
+  <si>
+    <t>10,427.77</t>
+  </si>
+  <si>
+    <t>11,249.94</t>
+  </si>
+  <si>
+    <t>10,892.01</t>
+  </si>
+  <si>
+    <t>10,479.86</t>
+  </si>
+  <si>
+    <t>11,304.15</t>
+  </si>
+  <si>
+    <t>10,995.25</t>
+  </si>
+  <si>
+    <t>10,581.98</t>
+  </si>
+  <si>
+    <t>11,408.52</t>
+  </si>
+  <si>
+    <t>10,997.81</t>
+  </si>
+  <si>
+    <t>10,583.35</t>
+  </si>
+  <si>
+    <t>11,412.27</t>
+  </si>
+  <si>
+    <t>10,896.71</t>
+  </si>
+  <si>
+    <t>10,480.99</t>
+  </si>
+  <si>
+    <t>11,312.43</t>
+  </si>
+  <si>
+    <t>Tendencia polinomial grado 6</t>
+  </si>
+  <si>
+    <t>Tendencia con término (x⁶)</t>
+  </si>
+  <si>
+    <t>Aumenta la capacidad de ajuste al permitir una tendencia más flexible, aunque puede acercarse al sobreajuste.</t>
+  </si>
+  <si>
+    <t>La estacionalidad por sí sola no explica bien el comportamiento global de la serie.</t>
+  </si>
+  <si>
+    <t>Supuesto</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>p-valor</t>
+  </si>
+  <si>
+    <t>Conclusión</t>
+  </si>
+  <si>
+    <t>Autocorrelación</t>
+  </si>
+  <si>
+    <t>Ljung-Box</t>
+  </si>
+  <si>
+    <t>1.29e-30</t>
+  </si>
+  <si>
+    <t>Hay autocorrelación</t>
+  </si>
+  <si>
+    <t>Heteroscedasticidad</t>
+  </si>
+  <si>
+    <t>Ljung-Box (res²), Breusch-Pagan</t>
+  </si>
+  <si>
+    <t>&lt; 0.05 / 0.032</t>
+  </si>
+  <si>
+    <t>Hay heteroscedasticidad</t>
+  </si>
+  <si>
+    <t>Normalidad</t>
+  </si>
+  <si>
+    <t>Shapiro-Wilk, Jarque-Bera</t>
+  </si>
+  <si>
+    <t>0.0056 / 0.014</t>
+  </si>
+  <si>
+    <t>No hay normalidad</t>
   </si>
 </sst>
 </file>
@@ -385,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -411,14 +522,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,19 +875,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B6C11-13F9-4C03-BFC2-EFBD0D58981C}">
-  <dimension ref="C9:K113"/>
+  <dimension ref="C9:K114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G101" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M104" sqref="M104"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.08984375" customWidth="1"/>
     <col min="7" max="7" width="60.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.7265625" customWidth="1"/>
-    <col min="9" max="11" width="18.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="4:5" x14ac:dyDescent="0.35">
@@ -861,7 +982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:8" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C31" s="1" t="s">
         <v>20</v>
       </c>
@@ -875,92 +996,92 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:8" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="5">
         <v>43647</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="H32" t="e">
         <f>F32-D32</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C33" s="5">
         <v>43678</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C34" s="5">
         <v>43709</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C35" s="5">
         <v>43739</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C36" s="5">
         <v>43770</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="5">
         <v>43800</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.35">
@@ -1181,162 +1302,232 @@
         <v>66</v>
       </c>
       <c r="E69" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="70" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C70" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" ht="29" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C71" s="3" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C72" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C73" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="8:11" x14ac:dyDescent="0.35">
+      <c r="H82" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="83" spans="8:11" x14ac:dyDescent="0.35">
+      <c r="H83" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I83" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J83" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="K83" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="8:11" x14ac:dyDescent="0.35">
+      <c r="H84" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I84" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J84" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="K84" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="8:11" x14ac:dyDescent="0.35">
+      <c r="H85" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="I85" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K85" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="105" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I105" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J105" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K105" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I106" s="10">
+        <v>2</v>
+      </c>
+      <c r="J106" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K106" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D72" s="2" t="s">
+    </row>
+    <row r="107" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I107" s="10">
+        <v>3</v>
+      </c>
+      <c r="J107" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="K107" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F72" s="2" t="s">
+    </row>
+    <row r="108" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I108" s="10">
+        <v>4</v>
+      </c>
+      <c r="J108" s="10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="104" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I104" s="11" t="s">
+      <c r="K108" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J104" s="11" t="s">
+    </row>
+    <row r="109" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I109" s="10">
+        <v>5</v>
+      </c>
+      <c r="J109" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="K104" s="11" t="s">
+      <c r="K109" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="105" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I105" s="9">
-        <v>2</v>
-      </c>
-      <c r="J105" s="9" t="s">
+    <row r="110" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I110" s="11">
+        <v>6</v>
+      </c>
+      <c r="J110" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="K105" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="106" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I106" s="9">
-        <v>3</v>
-      </c>
-      <c r="J106" s="9" t="s">
+      <c r="K110" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="K106" s="9" t="s">
+    </row>
+    <row r="111" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I111" s="10">
+        <v>7</v>
+      </c>
+      <c r="J111" s="12">
+        <v>-43530</v>
+      </c>
+      <c r="K111" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I107" s="9">
-        <v>4</v>
-      </c>
-      <c r="J107" s="9" t="s">
+    <row r="112" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I112" s="10">
+        <v>8</v>
+      </c>
+      <c r="J112" s="12">
+        <v>-357405</v>
+      </c>
+      <c r="K112" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="K107" s="9" t="s">
+    </row>
+    <row r="113" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I113" s="10">
+        <v>9</v>
+      </c>
+      <c r="J113" s="12">
+        <v>-370772</v>
+      </c>
+      <c r="K113" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="108" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I108" s="9">
-        <v>5</v>
-      </c>
-      <c r="J108" s="9" t="s">
+    <row r="114" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I114" s="10">
+        <v>10</v>
+      </c>
+      <c r="J114" s="12">
+        <v>-381932</v>
+      </c>
+      <c r="K114" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="K108" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="109" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I109" s="11">
-        <v>6</v>
-      </c>
-      <c r="J109" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="K109" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="110" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I110" s="9">
-        <v>7</v>
-      </c>
-      <c r="J110" s="10">
-        <v>-45481</v>
-      </c>
-      <c r="K110" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="111" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I111" s="9">
-        <v>8</v>
-      </c>
-      <c r="J111" s="10">
-        <v>-364369</v>
-      </c>
-      <c r="K111" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="112" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I112" s="9">
-        <v>9</v>
-      </c>
-      <c r="J112" s="10">
-        <v>-378056</v>
-      </c>
-      <c r="K112" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="113" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I113" s="9">
-        <v>10</v>
-      </c>
-      <c r="J113" s="10">
-        <v>-389498</v>
-      </c>
-      <c r="K113" s="9" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>